<commit_message>
meta: update preview images
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/line-chart/line-chart.xlsx
+++ b/_examples/spreadsheet/line-chart/line-chart.xlsx
@@ -233,7 +233,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="0"/>
+        <c:crossAx val="449512514"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -261,7 +261,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="0"/>
+        <c:crossAx val="1891972126"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
       </c:catAx>
     </c:plotArea>
@@ -290,25 +291,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff/>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff/>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff/>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff/>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm/>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" uri="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>

</xml_diff>